<commit_message>
Generalising plotting options and improving quality of figures
Part way through the task, much still to be done.
</commit_message>
<xml_diff>
--- a/notebooks/ModelInputs/Old_Param_files/parameters_v1.xlsx
+++ b/notebooks/ModelInputs/Old_Param_files/parameters_v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="18195" windowHeight="11700"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="18195" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LU" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="183">
   <si>
     <t>Param</t>
   </si>
@@ -570,9 +570,6 @@
   </si>
   <si>
     <t>m s2/kg</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>K_erosion</t>
@@ -1243,7 +1240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -1408,13 +1405,13 @@
         <v>92</v>
       </c>
       <c r="B7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" t="s">
         <v>181</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>182</v>
-      </c>
-      <c r="D7" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1442,10 +1439,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,7 +1604,7 @@
         <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1627,7 +1624,7 @@
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1647,7 +1644,7 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1672,19 +1669,19 @@
         <v>92</v>
       </c>
       <c r="B13" s="41" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" t="s">
         <v>177</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>178</v>
-      </c>
-      <c r="D13" t="s">
-        <v>179</v>
       </c>
       <c r="E13">
         <v>0.02</v>
       </c>
       <c r="F13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1719,11 +1716,6 @@
       </c>
       <c r="E15" s="3">
         <v>0.26</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>